<commit_message>
from pc to laptop.  I wrote this on my pc
</commit_message>
<xml_diff>
--- a/cmake-build-debug/Graphed Data/bubbleSortFile.xlsx
+++ b/cmake-build-debug/Graphed Data/bubbleSortFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amccm\CLionProjects\Project_4\cmake-build-debug\Graphed Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A5D29C-7E83-4588-9C08-BE400AF44A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B21D0E-2C06-4E81-9D9F-E6488DA9C192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="3120" windowWidth="21540" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21540" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bubbleSortFile" sheetId="1" r:id="rId1"/>
@@ -649,9 +649,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -668,15 +667,17 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>bubbleSortFile!$A$2:$A$11</c:f>
@@ -755,9 +756,10 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9757-44A2-AD03-73DAB7758570}"/>
+              <c16:uniqueId val="{00000000-0044-44EF-B532-1C0A2E8303D6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -776,15 +778,17 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>bubbleSortFile!$A$2:$A$11</c:f>
@@ -863,9 +867,10 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9757-44A2-AD03-73DAB7758570}"/>
+              <c16:uniqueId val="{00000001-0044-44EF-B532-1C0A2E8303D6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -877,13 +882,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="2036568511"/>
-        <c:axId val="2036566847"/>
-      </c:barChart>
+        <c:smooth val="0"/>
+        <c:axId val="1345079935"/>
+        <c:axId val="1345077855"/>
+      </c:lineChart>
       <c:catAx>
-        <c:axId val="2036568511"/>
+        <c:axId val="1345079935"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -981,7 +985,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2036566847"/>
+        <c:crossAx val="1345077855"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -989,7 +993,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2036566847"/>
+        <c:axId val="1345077855"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1030,13 +1034,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Reads</a:t>
+                  <a:t>Reads and Writes</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> and Writes</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1100,7 +1099,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2036568511"/>
+        <c:crossAx val="1345079935"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1221,7 +1220,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1329,6 +1328,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1339,6 +1343,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -1370,6 +1379,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1728,22 +1740,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:colOff>519112</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:colOff>214312</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCB9B36D-79C5-4544-A339-EBE0CBF8C22F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36A228CA-5778-4B46-B25D-A3A0C05AC094}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2063,7 +2075,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>